<commit_message>
File differences test completed.
</commit_message>
<xml_diff>
--- a/file1.xlsx
+++ b/file1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miket/Downloads/Portfolio_Projects/cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBF085B-05F7-9547-8F8A-D6D7AD47B82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566A69DE-03FD-3143-9654-7265A113DEC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{0851F0FD-89FF-1948-B25E-60702C1D489B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Adam</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>Daniel</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -419,43 +434,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EBFAE1-BC30-4449-8674-E31595D30E86}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>